<commit_message>
Updated all tutorials to openpyxl.
</commit_message>
<xml_diff>
--- a/docs/Files/ManufacturingYieldloss_Tutorial.xlsx
+++ b/docs/Files/ManufacturingYieldloss_Tutorial.xlsx
@@ -5,28 +5,22 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spauliuk\FILES\ARBEIT\Software\IPython\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spauliuk.AD\FILES\ARBEIT\PROJECTS\ODYM-RECC\ODYM_Model\docs\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="90" windowWidth="16335" windowHeight="10830"/>
   </bookViews>
   <sheets>
-    <sheet name="Cover" sheetId="6" r:id="rId1"/>
-    <sheet name="Value_Master" sheetId="1" r:id="rId2"/>
+    <sheet name="Cover" sheetId="7" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="96">
-  <si>
-    <t>V0.1</t>
-  </si>
-  <si>
-    <t>None (define indicator in general system definition later)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="101">
   <si>
     <t>None</t>
   </si>
@@ -41,21 +35,6 @@
   </si>
   <si>
     <t>Pauliuk</t>
-  </si>
-  <si>
-    <t>Table</t>
-  </si>
-  <si>
-    <t>RowIndices</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># Specify indices in order of appearance in data table. </t>
-  </si>
-  <si>
-    <t>ColumnIndices</t>
-  </si>
-  <si>
-    <t>ValueInfo</t>
   </si>
   <si>
     <t># Specify the version number of the formatting used for this file</t>
@@ -97,9 +76,6 @@
     <t># Points to processes and flows in a general system definition, optional</t>
   </si>
   <si>
-    <t># ID of dataset, optional</t>
-  </si>
-  <si>
     <t># UUID of dataset, can be generated manually, for archiving and reference purposes</t>
   </si>
   <si>
@@ -115,64 +91,16 @@
     <t># Version number of dataset</t>
   </si>
   <si>
-    <t># Version number of classifications used for this dataset</t>
-  </si>
-  <si>
     <t>Dataset_RecordType</t>
-  </si>
-  <si>
-    <t>*) Fields highlighted in grey are mandatory. Order of fields and field naming is fixed, do not change!</t>
-  </si>
-  <si>
-    <t>RowIndices_Meaning</t>
-  </si>
-  <si>
-    <t>ColumnIndices_Meaning</t>
-  </si>
-  <si>
-    <t># Describe meaning of each row index</t>
-  </si>
-  <si>
-    <t># Describe meaning of each column index</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>ValueInfoComment</t>
-  </si>
-  <si>
     <t># Two types are supported: list and table</t>
   </si>
   <si>
-    <t>RowNumbers</t>
-  </si>
-  <si>
-    <t>ColumnNumbers</t>
-  </si>
-  <si>
-    <t># Specify the total number of data columns (data table width)</t>
-  </si>
-  <si>
-    <t># Specify the total number of data rows (data table height)</t>
-  </si>
-  <si>
     <t>GLOBAL</t>
-  </si>
-  <si>
-    <t># Unit of dataset: Col B: GLOBAL: cf. UNITS sheet in classification master file, LIST: As separate Column in listed data. SHEET: as separate sheet in tabular data. Col C: Unit, composed of elements as definined in UNITS table, separated by * / and (). Col D: Comment/Description</t>
-  </si>
-  <si>
-    <t>Value_Master</t>
-  </si>
-  <si>
-    <t># Specify the different quantification layers given: Value, Error, etc, or different scenarios. Must be identical to sheet names following. Specific sheet names (Value_Master, Unit, LowerBound, UpperBound, STD, etc. will have predefined meanings in the future.)</t>
-  </si>
-  <si>
-    <t># Describe the different quantification layers</t>
-  </si>
-  <si>
-    <t>ODYM Parameter File*</t>
   </si>
   <si>
     <t>Manufacturing yield loss</t>
@@ -203,9 +131,6 @@
   </si>
   <si>
     <t>waste and scrap groups</t>
-  </si>
-  <si>
-    <t>Mean value of yield loss parameter</t>
   </si>
   <si>
     <t>ManufacturingYieldloss_Tutorial</t>
@@ -307,14 +232,104 @@
     <t>Default is 100% loss in cases where material does not enter product</t>
   </si>
   <si>
-    <t>DUMMY data</t>
+    <t>ODYM-RECC Parameter File</t>
+  </si>
+  <si>
+    <t># Fields highlighted in grey are mandatory. Fields highlighted in blue are linked to other tables and databases. Order of fields and field naming is fixed, do not change!</t>
+  </si>
+  <si>
+    <t>V0.2</t>
+  </si>
+  <si>
+    <t>Unit_nominator</t>
+  </si>
+  <si>
+    <t>Unit_denominator</t>
+  </si>
+  <si>
+    <t># Unit of dataset, cf. UNITS sheet in classification master file, GLOBAL, LIST, or TABLE</t>
+  </si>
+  <si>
+    <t>Dataset_Uncertainty</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t># Uncertainty in form of stats_array string (http://stats-arrays.readthedocs.io/en/latest/), GLOBAL, LIST, or TABLE</t>
+  </si>
+  <si>
+    <t>Dataset_Comment</t>
+  </si>
+  <si>
+    <t>TABLE</t>
+  </si>
+  <si>
+    <t># Comment, GLOBAL, LIST, or TABLE</t>
+  </si>
+  <si>
+    <t># ID of dataset, optional, establish link to IEDI</t>
+  </si>
+  <si>
+    <t>V1.0</t>
+  </si>
+  <si>
+    <t># Version number of classifications used for this dataset. Points to ODYM classification file with name name.</t>
+  </si>
+  <si>
+    <t>[Empty on purpose]</t>
+  </si>
+  <si>
+    <t>No_Rows</t>
+  </si>
+  <si>
+    <t>No_Cols</t>
+  </si>
+  <si>
+    <t>Row Aspects classification</t>
+  </si>
+  <si>
+    <t>Row Aspects_Meaning</t>
+  </si>
+  <si>
+    <t>Col Aspects classification</t>
+  </si>
+  <si>
+    <t>Col Aspects_Meaning</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>DATA_Info</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Vehicle stock</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Row and col(umn) aspects: Specify row and column aspects in order of appearance in data table. </t>
+  </si>
+  <si>
+    <t># Row and col(umn) aspects_Meaning: Describe meaning of each row and column aspect</t>
+  </si>
+  <si>
+    <t># DATA: Specify the different quantification layers given: Value, Error, etc, or different scenarios. Must be identical to data sheet names</t>
+  </si>
+  <si>
+    <t># DATA_Info: Describe each data layer</t>
+  </si>
+  <si>
+    <t>Manufacturing sector</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -330,13 +345,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -360,7 +368,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -370,6 +378,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -386,23 +400,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -421,7 +444,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -683,419 +706,511 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.42578125" style="7"/>
-    <col min="7" max="8" width="2.7109375" style="7" customWidth="1"/>
-    <col min="9" max="9" width="2.85546875" style="7" customWidth="1"/>
-    <col min="10" max="10" width="3" style="7" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="7"/>
+    <col min="1" max="1" width="34.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
+    <col min="3" max="3" width="15.796875" customWidth="1"/>
+    <col min="4" max="4" width="17.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
-        <v>50</v>
+        <v>70</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="14">
+        <v>1</v>
+      </c>
+      <c r="D5" s="14">
+        <v>1</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A6" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A7" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>12</v>
+      <c r="B14" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="15" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>22</v>
+      <c r="B15" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" s="7" t="s">
+    <row r="16" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A16" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A17" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A18" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A19" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="12"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A20" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="12"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="B21" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="17">
+        <v>80</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F21" s="17">
+        <v>10</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="11">
-        <v>1</v>
-      </c>
-      <c r="D5" s="7">
-        <v>1</v>
-      </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>46</v>
-      </c>
+    <row r="22" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A22" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="7"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L6" s="7" t="s">
+    <row r="23" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A23" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G23" s="8" t="s">
         <v>24</v>
       </c>
+      <c r="H23" s="7" t="s">
+        <v>96</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>25</v>
+    <row r="24" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A24" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>26</v>
+    <row r="25" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>27</v>
+    <row r="26" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>28</v>
-      </c>
+    <row r="27" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" s="7"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="7">
-        <v>80</v>
-      </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L17" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L18" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="7">
-        <v>10</v>
-      </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L20" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L21" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L22" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
-        <v>33</v>
-      </c>
+    <row r="28" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1113,60 +1228,60 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="60" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" style="13" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="13" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="13" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="13" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="13" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" style="13" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="13" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13" style="13" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="13"/>
+    <col min="1" max="1" width="22.1328125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="60" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" style="11" customWidth="1"/>
+    <col min="4" max="4" width="11.265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.59765625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="12.73046875" style="11" customWidth="1"/>
+    <col min="7" max="7" width="13.86328125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="13.59765625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="14.1328125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="13.59765625" style="11" customWidth="1"/>
+    <col min="11" max="11" width="10.3984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13" style="11" customWidth="1"/>
+    <col min="13" max="16384" width="11.3984375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
-        <v>94</v>
+    <row r="1" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A1" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -1318,12 +1433,12 @@
       <c r="FD1" s="2"/>
       <c r="FE1" s="2"/>
     </row>
-    <row r="2" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>63</v>
+    <row r="2" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A2" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -1505,12 +1620,12 @@
       <c r="FD2" s="2"/>
       <c r="FE2" s="2"/>
     </row>
-    <row r="3" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>64</v>
+    <row r="3" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A3" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -1692,12 +1807,12 @@
       <c r="FD3" s="2"/>
       <c r="FE3" s="2"/>
     </row>
-    <row r="4" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>65</v>
+    <row r="4" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A4" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="C4" s="2">
         <v>0.05</v>
@@ -1879,12 +1994,12 @@
       <c r="FD4" s="2"/>
       <c r="FE4" s="2"/>
     </row>
-    <row r="5" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>66</v>
+    <row r="5" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A5" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="C5" s="2">
         <v>0.08</v>
@@ -2066,12 +2181,12 @@
       <c r="FD5" s="2"/>
       <c r="FE5" s="2"/>
     </row>
-    <row r="6" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>67</v>
+    <row r="6" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A6" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -2253,12 +2368,12 @@
       <c r="FD6" s="2"/>
       <c r="FE6" s="2"/>
     </row>
-    <row r="7" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>68</v>
+    <row r="7" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A7" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -2440,12 +2555,12 @@
       <c r="FD7" s="2"/>
       <c r="FE7" s="2"/>
     </row>
-    <row r="8" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>69</v>
+    <row r="8" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A8" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
@@ -2627,12 +2742,12 @@
       <c r="FD8" s="2"/>
       <c r="FE8" s="2"/>
     </row>
-    <row r="9" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>70</v>
+    <row r="9" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A9" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -2814,12 +2929,12 @@
       <c r="FD9" s="2"/>
       <c r="FE9" s="2"/>
     </row>
-    <row r="10" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>71</v>
+    <row r="10" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A10" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -3001,12 +3116,12 @@
       <c r="FD10" s="2"/>
       <c r="FE10" s="2"/>
     </row>
-    <row r="11" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>72</v>
+    <row r="11" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A11" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
@@ -3188,12 +3303,12 @@
       <c r="FD11" s="2"/>
       <c r="FE11" s="2"/>
     </row>
-    <row r="12" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>73</v>
+    <row r="12" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A12" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="C12" s="2">
         <v>1</v>
@@ -3375,12 +3490,12 @@
       <c r="FD12" s="2"/>
       <c r="FE12" s="2"/>
     </row>
-    <row r="13" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>74</v>
+    <row r="13" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A13" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="C13" s="2">
         <v>1</v>
@@ -3562,12 +3677,12 @@
       <c r="FD13" s="2"/>
       <c r="FE13" s="2"/>
     </row>
-    <row r="14" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>75</v>
+    <row r="14" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A14" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="C14" s="2">
         <v>1</v>
@@ -3749,12 +3864,12 @@
       <c r="FD14" s="2"/>
       <c r="FE14" s="2"/>
     </row>
-    <row r="15" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>76</v>
+    <row r="15" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="C15" s="2">
         <v>1</v>
@@ -3936,12 +4051,12 @@
       <c r="FD15" s="2"/>
       <c r="FE15" s="2"/>
     </row>
-    <row r="16" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>77</v>
+    <row r="16" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A16" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="C16" s="2">
         <v>1</v>
@@ -4123,12 +4238,12 @@
       <c r="FD16" s="2"/>
       <c r="FE16" s="2"/>
     </row>
-    <row r="17" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>78</v>
+    <row r="17" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A17" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="C17" s="2">
         <v>1</v>
@@ -4310,12 +4425,12 @@
       <c r="FD17" s="2"/>
       <c r="FE17" s="2"/>
     </row>
-    <row r="18" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>63</v>
+        <v>55</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="C18" s="2">
         <v>0</v>
@@ -4497,12 +4612,12 @@
       <c r="FD18" s="2"/>
       <c r="FE18" s="2"/>
     </row>
-    <row r="19" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>64</v>
+        <v>55</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C19" s="2">
         <v>0</v>
@@ -4684,12 +4799,12 @@
       <c r="FD19" s="2"/>
       <c r="FE19" s="2"/>
     </row>
-    <row r="20" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>65</v>
+        <v>55</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="C20" s="2">
         <v>0</v>
@@ -4871,12 +4986,12 @@
       <c r="FD20" s="2"/>
       <c r="FE20" s="2"/>
     </row>
-    <row r="21" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>66</v>
+        <v>55</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="C21" s="2">
         <v>0</v>
@@ -5058,12 +5173,12 @@
       <c r="FD21" s="2"/>
       <c r="FE21" s="2"/>
     </row>
-    <row r="22" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>67</v>
+        <v>55</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="C22" s="2">
         <v>0</v>
@@ -5245,12 +5360,12 @@
       <c r="FD22" s="2"/>
       <c r="FE22" s="2"/>
     </row>
-    <row r="23" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>68</v>
+        <v>55</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="C23" s="2">
         <v>0</v>
@@ -5432,12 +5547,12 @@
       <c r="FD23" s="2"/>
       <c r="FE23" s="2"/>
     </row>
-    <row r="24" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>69</v>
+        <v>55</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="C24" s="2">
         <v>0</v>
@@ -5619,12 +5734,12 @@
       <c r="FD24" s="2"/>
       <c r="FE24" s="2"/>
     </row>
-    <row r="25" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>70</v>
+        <v>55</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="C25" s="2">
         <v>0</v>
@@ -5806,12 +5921,12 @@
       <c r="FD25" s="2"/>
       <c r="FE25" s="2"/>
     </row>
-    <row r="26" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>71</v>
+        <v>55</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="C26" s="2">
         <v>0</v>
@@ -5993,12 +6108,12 @@
       <c r="FD26" s="2"/>
       <c r="FE26" s="2"/>
     </row>
-    <row r="27" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>72</v>
+        <v>55</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="C27" s="2">
         <v>0</v>
@@ -6180,12 +6295,12 @@
       <c r="FD27" s="2"/>
       <c r="FE27" s="2"/>
     </row>
-    <row r="28" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>73</v>
+        <v>55</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="C28" s="2">
         <v>0</v>
@@ -6367,12 +6482,12 @@
       <c r="FD28" s="2"/>
       <c r="FE28" s="2"/>
     </row>
-    <row r="29" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>74</v>
+        <v>55</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="C29" s="2">
         <v>0</v>
@@ -6554,12 +6669,12 @@
       <c r="FD29" s="2"/>
       <c r="FE29" s="2"/>
     </row>
-    <row r="30" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>75</v>
+        <v>55</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="C30" s="2">
         <v>0</v>
@@ -6741,12 +6856,12 @@
       <c r="FD30" s="2"/>
       <c r="FE30" s="2"/>
     </row>
-    <row r="31" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>76</v>
+        <v>55</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="C31" s="2">
         <v>0</v>
@@ -6928,12 +7043,12 @@
       <c r="FD31" s="2"/>
       <c r="FE31" s="2"/>
     </row>
-    <row r="32" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>77</v>
+        <v>55</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="C32" s="2">
         <v>0</v>
@@ -7115,12 +7230,12 @@
       <c r="FD32" s="2"/>
       <c r="FE32" s="2"/>
     </row>
-    <row r="33" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>78</v>
+        <v>55</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="C33" s="2">
         <v>0</v>
@@ -7302,12 +7417,12 @@
       <c r="FD33" s="2"/>
       <c r="FE33" s="2"/>
     </row>
-    <row r="34" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>63</v>
+        <v>56</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="C34" s="2">
         <v>0</v>
@@ -7489,12 +7604,12 @@
       <c r="FD34" s="2"/>
       <c r="FE34" s="2"/>
     </row>
-    <row r="35" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>64</v>
+        <v>56</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C35" s="2">
         <v>0</v>
@@ -7676,12 +7791,12 @@
       <c r="FD35" s="2"/>
       <c r="FE35" s="2"/>
     </row>
-    <row r="36" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>65</v>
+        <v>56</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="C36" s="2">
         <v>0</v>
@@ -7863,12 +7978,12 @@
       <c r="FD36" s="2"/>
       <c r="FE36" s="2"/>
     </row>
-    <row r="37" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>66</v>
+        <v>56</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="C37" s="2">
         <v>0</v>
@@ -8050,12 +8165,12 @@
       <c r="FD37" s="2"/>
       <c r="FE37" s="2"/>
     </row>
-    <row r="38" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>67</v>
+        <v>56</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="C38" s="2">
         <v>0</v>
@@ -8237,12 +8352,12 @@
       <c r="FD38" s="2"/>
       <c r="FE38" s="2"/>
     </row>
-    <row r="39" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>68</v>
+        <v>56</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="C39" s="2">
         <v>0</v>
@@ -8424,12 +8539,12 @@
       <c r="FD39" s="2"/>
       <c r="FE39" s="2"/>
     </row>
-    <row r="40" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>69</v>
+        <v>56</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="C40" s="2">
         <v>0</v>
@@ -8611,12 +8726,12 @@
       <c r="FD40" s="2"/>
       <c r="FE40" s="2"/>
     </row>
-    <row r="41" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>70</v>
+        <v>56</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="C41" s="2">
         <v>0</v>
@@ -8798,12 +8913,12 @@
       <c r="FD41" s="2"/>
       <c r="FE41" s="2"/>
     </row>
-    <row r="42" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>71</v>
+        <v>56</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="C42" s="2">
         <v>0</v>
@@ -8985,12 +9100,12 @@
       <c r="FD42" s="2"/>
       <c r="FE42" s="2"/>
     </row>
-    <row r="43" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>72</v>
+        <v>56</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="C43" s="2">
         <v>0</v>
@@ -9172,12 +9287,12 @@
       <c r="FD43" s="2"/>
       <c r="FE43" s="2"/>
     </row>
-    <row r="44" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>73</v>
+        <v>56</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="C44" s="2">
         <v>0</v>
@@ -9359,12 +9474,12 @@
       <c r="FD44" s="2"/>
       <c r="FE44" s="2"/>
     </row>
-    <row r="45" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>74</v>
+        <v>56</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="C45" s="2">
         <v>0</v>
@@ -9546,12 +9661,12 @@
       <c r="FD45" s="2"/>
       <c r="FE45" s="2"/>
     </row>
-    <row r="46" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A46" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>75</v>
+        <v>56</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="C46" s="2">
         <v>0</v>
@@ -9733,12 +9848,12 @@
       <c r="FD46" s="2"/>
       <c r="FE46" s="2"/>
     </row>
-    <row r="47" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>76</v>
+        <v>56</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="C47" s="2">
         <v>0</v>
@@ -9920,12 +10035,12 @@
       <c r="FD47" s="2"/>
       <c r="FE47" s="2"/>
     </row>
-    <row r="48" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>77</v>
+        <v>56</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="C48" s="2">
         <v>0</v>
@@ -10107,12 +10222,12 @@
       <c r="FD48" s="2"/>
       <c r="FE48" s="2"/>
     </row>
-    <row r="49" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>78</v>
+        <v>56</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="C49" s="2">
         <v>0</v>
@@ -10294,12 +10409,12 @@
       <c r="FD49" s="2"/>
       <c r="FE49" s="2"/>
     </row>
-    <row r="50" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>63</v>
+        <v>57</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="C50" s="2">
         <v>0</v>
@@ -10481,12 +10596,12 @@
       <c r="FD50" s="2"/>
       <c r="FE50" s="2"/>
     </row>
-    <row r="51" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A51" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>64</v>
+        <v>57</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C51" s="2">
         <v>0</v>
@@ -10668,12 +10783,12 @@
       <c r="FD51" s="2"/>
       <c r="FE51" s="2"/>
     </row>
-    <row r="52" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>65</v>
+        <v>57</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="C52" s="2">
         <v>0</v>
@@ -10855,12 +10970,12 @@
       <c r="FD52" s="2"/>
       <c r="FE52" s="2"/>
     </row>
-    <row r="53" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A53" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>66</v>
+        <v>57</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="C53" s="2">
         <v>0</v>
@@ -11042,12 +11157,12 @@
       <c r="FD53" s="2"/>
       <c r="FE53" s="2"/>
     </row>
-    <row r="54" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A54" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>67</v>
+        <v>57</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="C54" s="2">
         <v>0</v>
@@ -11229,12 +11344,12 @@
       <c r="FD54" s="2"/>
       <c r="FE54" s="2"/>
     </row>
-    <row r="55" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A55" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B55" s="12" t="s">
-        <v>68</v>
+        <v>57</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="C55" s="2">
         <v>0</v>
@@ -11416,12 +11531,12 @@
       <c r="FD55" s="2"/>
       <c r="FE55" s="2"/>
     </row>
-    <row r="56" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A56" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B56" s="12" t="s">
-        <v>69</v>
+        <v>57</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="C56" s="2">
         <v>0</v>
@@ -11603,12 +11718,12 @@
       <c r="FD56" s="2"/>
       <c r="FE56" s="2"/>
     </row>
-    <row r="57" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A57" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B57" s="12" t="s">
-        <v>70</v>
+        <v>57</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="C57" s="2">
         <v>0</v>
@@ -11790,12 +11905,12 @@
       <c r="FD57" s="2"/>
       <c r="FE57" s="2"/>
     </row>
-    <row r="58" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A58" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>71</v>
+        <v>57</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="C58" s="2">
         <v>0</v>
@@ -11977,12 +12092,12 @@
       <c r="FD58" s="2"/>
       <c r="FE58" s="2"/>
     </row>
-    <row r="59" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A59" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B59" s="12" t="s">
-        <v>72</v>
+        <v>57</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="C59" s="2">
         <v>0</v>
@@ -12164,12 +12279,12 @@
       <c r="FD59" s="2"/>
       <c r="FE59" s="2"/>
     </row>
-    <row r="60" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A60" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B60" s="12" t="s">
-        <v>73</v>
+        <v>57</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="C60" s="2">
         <v>0</v>
@@ -12351,12 +12466,12 @@
       <c r="FD60" s="2"/>
       <c r="FE60" s="2"/>
     </row>
-    <row r="61" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A61" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B61" s="12" t="s">
-        <v>74</v>
+        <v>57</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="C61" s="2">
         <v>0</v>
@@ -12538,12 +12653,12 @@
       <c r="FD61" s="2"/>
       <c r="FE61" s="2"/>
     </row>
-    <row r="62" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A62" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>75</v>
+        <v>57</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="C62" s="2">
         <v>0</v>
@@ -12725,12 +12840,12 @@
       <c r="FD62" s="2"/>
       <c r="FE62" s="2"/>
     </row>
-    <row r="63" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A63" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B63" s="12" t="s">
-        <v>76</v>
+        <v>57</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="C63" s="2">
         <v>0</v>
@@ -12912,12 +13027,12 @@
       <c r="FD63" s="2"/>
       <c r="FE63" s="2"/>
     </row>
-    <row r="64" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A64" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B64" s="12" t="s">
-        <v>77</v>
+        <v>57</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="C64" s="2">
         <v>0</v>
@@ -13099,12 +13214,12 @@
       <c r="FD64" s="2"/>
       <c r="FE64" s="2"/>
     </row>
-    <row r="65" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A65" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B65" s="12" t="s">
-        <v>78</v>
+        <v>57</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="C65" s="2">
         <v>0</v>
@@ -13286,12 +13401,12 @@
       <c r="FD65" s="2"/>
       <c r="FE65" s="2"/>
     </row>
-    <row r="66" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A66" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B66" s="12" t="s">
-        <v>63</v>
+    <row r="66" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A66" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="C66" s="2">
         <v>0</v>
@@ -13473,12 +13588,12 @@
       <c r="FD66" s="2"/>
       <c r="FE66" s="2"/>
     </row>
-    <row r="67" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A67" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B67" s="12" t="s">
-        <v>64</v>
+    <row r="67" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A67" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C67" s="2">
         <v>0</v>
@@ -13660,12 +13775,12 @@
       <c r="FD67" s="2"/>
       <c r="FE67" s="2"/>
     </row>
-    <row r="68" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A68" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B68" s="12" t="s">
-        <v>65</v>
+    <row r="68" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A68" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="C68" s="2">
         <v>0</v>
@@ -13847,12 +13962,12 @@
       <c r="FD68" s="2"/>
       <c r="FE68" s="2"/>
     </row>
-    <row r="69" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A69" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B69" s="12" t="s">
-        <v>66</v>
+    <row r="69" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A69" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="C69" s="2">
         <v>0</v>
@@ -14034,12 +14149,12 @@
       <c r="FD69" s="2"/>
       <c r="FE69" s="2"/>
     </row>
-    <row r="70" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A70" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B70" s="12" t="s">
-        <v>67</v>
+    <row r="70" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A70" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="C70" s="2">
         <v>0</v>
@@ -14221,12 +14336,12 @@
       <c r="FD70" s="2"/>
       <c r="FE70" s="2"/>
     </row>
-    <row r="71" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A71" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B71" s="12" t="s">
-        <v>68</v>
+    <row r="71" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A71" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="C71" s="2">
         <v>0</v>
@@ -14408,12 +14523,12 @@
       <c r="FD71" s="2"/>
       <c r="FE71" s="2"/>
     </row>
-    <row r="72" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A72" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B72" s="12" t="s">
-        <v>69</v>
+    <row r="72" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A72" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="C72" s="2">
         <v>0</v>
@@ -14595,12 +14710,12 @@
       <c r="FD72" s="2"/>
       <c r="FE72" s="2"/>
     </row>
-    <row r="73" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A73" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B73" s="12" t="s">
-        <v>70</v>
+    <row r="73" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A73" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="C73" s="2">
         <v>0</v>
@@ -14782,12 +14897,12 @@
       <c r="FD73" s="2"/>
       <c r="FE73" s="2"/>
     </row>
-    <row r="74" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A74" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B74" s="12" t="s">
-        <v>71</v>
+    <row r="74" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A74" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="C74" s="2">
         <v>0</v>
@@ -14969,12 +15084,12 @@
       <c r="FD74" s="2"/>
       <c r="FE74" s="2"/>
     </row>
-    <row r="75" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A75" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B75" s="12" t="s">
-        <v>72</v>
+    <row r="75" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A75" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="C75" s="2">
         <v>0</v>
@@ -15156,12 +15271,12 @@
       <c r="FD75" s="2"/>
       <c r="FE75" s="2"/>
     </row>
-    <row r="76" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A76" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B76" s="12" t="s">
-        <v>73</v>
+    <row r="76" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A76" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="C76" s="2">
         <v>0</v>
@@ -15343,12 +15458,12 @@
       <c r="FD76" s="2"/>
       <c r="FE76" s="2"/>
     </row>
-    <row r="77" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A77" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B77" s="12" t="s">
-        <v>74</v>
+    <row r="77" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A77" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="C77" s="2">
         <v>0</v>
@@ -15530,12 +15645,12 @@
       <c r="FD77" s="2"/>
       <c r="FE77" s="2"/>
     </row>
-    <row r="78" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A78" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B78" s="12" t="s">
-        <v>75</v>
+    <row r="78" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A78" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B78" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="C78" s="2">
         <v>0</v>
@@ -15717,12 +15832,12 @@
       <c r="FD78" s="2"/>
       <c r="FE78" s="2"/>
     </row>
-    <row r="79" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A79" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B79" s="12" t="s">
-        <v>76</v>
+    <row r="79" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A79" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="C79" s="2">
         <v>0</v>
@@ -15904,12 +16019,12 @@
       <c r="FD79" s="2"/>
       <c r="FE79" s="2"/>
     </row>
-    <row r="80" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A80" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B80" s="12" t="s">
-        <v>77</v>
+    <row r="80" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A80" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="C80" s="2">
         <v>0</v>
@@ -16091,12 +16206,12 @@
       <c r="FD80" s="2"/>
       <c r="FE80" s="2"/>
     </row>
-    <row r="81" spans="1:161" x14ac:dyDescent="0.2">
-      <c r="A81" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B81" s="12" t="s">
-        <v>78</v>
+    <row r="81" spans="1:161" x14ac:dyDescent="0.4">
+      <c r="A81" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="C81" s="2">
         <v>0</v>
@@ -16278,7 +16393,7 @@
       <c r="FD81" s="2"/>
       <c r="FE81" s="2"/>
     </row>
-    <row r="82" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="2"/>
@@ -16441,7 +16556,7 @@
       <c r="FD82" s="2"/>
       <c r="FE82" s="2"/>
     </row>
-    <row r="83" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="2"/>
@@ -16604,7 +16719,7 @@
       <c r="FD83" s="2"/>
       <c r="FE83" s="2"/>
     </row>
-    <row r="84" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="2"/>
@@ -16767,7 +16882,7 @@
       <c r="FD84" s="2"/>
       <c r="FE84" s="2"/>
     </row>
-    <row r="85" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="2"/>
@@ -16930,7 +17045,7 @@
       <c r="FD85" s="2"/>
       <c r="FE85" s="2"/>
     </row>
-    <row r="86" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="2"/>
@@ -17093,7 +17208,7 @@
       <c r="FD86" s="2"/>
       <c r="FE86" s="2"/>
     </row>
-    <row r="87" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="2"/>
@@ -17256,7 +17371,7 @@
       <c r="FD87" s="2"/>
       <c r="FE87" s="2"/>
     </row>
-    <row r="88" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="2"/>
@@ -17419,7 +17534,7 @@
       <c r="FD88" s="2"/>
       <c r="FE88" s="2"/>
     </row>
-    <row r="89" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="2"/>
@@ -17582,7 +17697,7 @@
       <c r="FD89" s="2"/>
       <c r="FE89" s="2"/>
     </row>
-    <row r="90" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="2"/>
@@ -17745,7 +17860,7 @@
       <c r="FD90" s="2"/>
       <c r="FE90" s="2"/>
     </row>
-    <row r="91" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="2"/>
@@ -17908,7 +18023,7 @@
       <c r="FD91" s="2"/>
       <c r="FE91" s="2"/>
     </row>
-    <row r="92" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="2"/>
@@ -18071,7 +18186,7 @@
       <c r="FD92" s="2"/>
       <c r="FE92" s="2"/>
     </row>
-    <row r="93" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="2"/>
@@ -18234,7 +18349,7 @@
       <c r="FD93" s="2"/>
       <c r="FE93" s="2"/>
     </row>
-    <row r="94" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="2"/>
@@ -18397,7 +18512,7 @@
       <c r="FD94" s="2"/>
       <c r="FE94" s="2"/>
     </row>
-    <row r="95" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="2"/>
@@ -18560,7 +18675,7 @@
       <c r="FD95" s="2"/>
       <c r="FE95" s="2"/>
     </row>
-    <row r="96" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="2"/>
@@ -18723,7 +18838,7 @@
       <c r="FD96" s="2"/>
       <c r="FE96" s="2"/>
     </row>
-    <row r="97" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="2"/>
@@ -18886,7 +19001,7 @@
       <c r="FD97" s="2"/>
       <c r="FE97" s="2"/>
     </row>
-    <row r="98" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="2"/>
@@ -19049,7 +19164,7 @@
       <c r="FD98" s="2"/>
       <c r="FE98" s="2"/>
     </row>
-    <row r="99" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="2"/>
@@ -19212,7 +19327,7 @@
       <c r="FD99" s="2"/>
       <c r="FE99" s="2"/>
     </row>
-    <row r="100" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="2"/>
@@ -19375,7 +19490,7 @@
       <c r="FD100" s="2"/>
       <c r="FE100" s="2"/>
     </row>
-    <row r="101" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="2"/>
@@ -19538,7 +19653,7 @@
       <c r="FD101" s="2"/>
       <c r="FE101" s="2"/>
     </row>
-    <row r="102" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="2"/>
@@ -19701,7 +19816,7 @@
       <c r="FD102" s="2"/>
       <c r="FE102" s="2"/>
     </row>
-    <row r="103" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="2"/>
@@ -19864,7 +19979,7 @@
       <c r="FD103" s="2"/>
       <c r="FE103" s="2"/>
     </row>
-    <row r="104" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="2"/>
@@ -20027,7 +20142,7 @@
       <c r="FD104" s="2"/>
       <c r="FE104" s="2"/>
     </row>
-    <row r="105" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="2"/>
@@ -20190,7 +20305,7 @@
       <c r="FD105" s="2"/>
       <c r="FE105" s="2"/>
     </row>
-    <row r="106" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="2"/>
@@ -20353,7 +20468,7 @@
       <c r="FD106" s="2"/>
       <c r="FE106" s="2"/>
     </row>
-    <row r="107" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="2"/>
@@ -20516,7 +20631,7 @@
       <c r="FD107" s="2"/>
       <c r="FE107" s="2"/>
     </row>
-    <row r="108" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="2"/>
@@ -20679,7 +20794,7 @@
       <c r="FD108" s="2"/>
       <c r="FE108" s="2"/>
     </row>
-    <row r="109" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="2"/>
@@ -20842,7 +20957,7 @@
       <c r="FD109" s="2"/>
       <c r="FE109" s="2"/>
     </row>
-    <row r="110" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="2"/>
@@ -21005,7 +21120,7 @@
       <c r="FD110" s="2"/>
       <c r="FE110" s="2"/>
     </row>
-    <row r="111" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="2"/>
@@ -21168,7 +21283,7 @@
       <c r="FD111" s="2"/>
       <c r="FE111" s="2"/>
     </row>
-    <row r="112" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="2"/>
@@ -21331,7 +21446,7 @@
       <c r="FD112" s="2"/>
       <c r="FE112" s="2"/>
     </row>
-    <row r="113" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="2"/>
@@ -21494,7 +21609,7 @@
       <c r="FD113" s="2"/>
       <c r="FE113" s="2"/>
     </row>
-    <row r="114" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="2"/>
@@ -21657,7 +21772,7 @@
       <c r="FD114" s="2"/>
       <c r="FE114" s="2"/>
     </row>
-    <row r="115" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="2"/>
@@ -21820,7 +21935,7 @@
       <c r="FD115" s="2"/>
       <c r="FE115" s="2"/>
     </row>
-    <row r="116" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="2"/>
@@ -21983,7 +22098,7 @@
       <c r="FD116" s="2"/>
       <c r="FE116" s="2"/>
     </row>
-    <row r="117" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="2"/>
@@ -22146,7 +22261,7 @@
       <c r="FD117" s="2"/>
       <c r="FE117" s="2"/>
     </row>
-    <row r="118" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="2"/>
@@ -22309,7 +22424,7 @@
       <c r="FD118" s="2"/>
       <c r="FE118" s="2"/>
     </row>
-    <row r="119" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="2"/>
@@ -22472,7 +22587,7 @@
       <c r="FD119" s="2"/>
       <c r="FE119" s="2"/>
     </row>
-    <row r="120" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="2"/>
@@ -22635,7 +22750,7 @@
       <c r="FD120" s="2"/>
       <c r="FE120" s="2"/>
     </row>
-    <row r="121" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="2"/>
@@ -22798,7 +22913,7 @@
       <c r="FD121" s="2"/>
       <c r="FE121" s="2"/>
     </row>
-    <row r="122" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="2"/>
@@ -22961,7 +23076,7 @@
       <c r="FD122" s="2"/>
       <c r="FE122" s="2"/>
     </row>
-    <row r="123" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="2"/>
@@ -23124,7 +23239,7 @@
       <c r="FD123" s="2"/>
       <c r="FE123" s="2"/>
     </row>
-    <row r="124" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="2"/>
@@ -23287,7 +23402,7 @@
       <c r="FD124" s="2"/>
       <c r="FE124" s="2"/>
     </row>
-    <row r="125" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="2"/>
@@ -23450,7 +23565,7 @@
       <c r="FD125" s="2"/>
       <c r="FE125" s="2"/>
     </row>
-    <row r="126" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="2"/>
@@ -23613,7 +23728,7 @@
       <c r="FD126" s="2"/>
       <c r="FE126" s="2"/>
     </row>
-    <row r="127" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="2"/>
@@ -23776,7 +23891,7 @@
       <c r="FD127" s="2"/>
       <c r="FE127" s="2"/>
     </row>
-    <row r="128" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="2"/>
@@ -23939,7 +24054,7 @@
       <c r="FD128" s="2"/>
       <c r="FE128" s="2"/>
     </row>
-    <row r="129" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="2"/>
@@ -24102,7 +24217,7 @@
       <c r="FD129" s="2"/>
       <c r="FE129" s="2"/>
     </row>
-    <row r="130" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="2"/>
@@ -24265,7 +24380,7 @@
       <c r="FD130" s="2"/>
       <c r="FE130" s="2"/>
     </row>
-    <row r="131" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="2"/>
@@ -24428,7 +24543,7 @@
       <c r="FD131" s="2"/>
       <c r="FE131" s="2"/>
     </row>
-    <row r="132" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="2"/>
@@ -24591,7 +24706,7 @@
       <c r="FD132" s="2"/>
       <c r="FE132" s="2"/>
     </row>
-    <row r="133" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="2"/>
@@ -24754,7 +24869,7 @@
       <c r="FD133" s="2"/>
       <c r="FE133" s="2"/>
     </row>
-    <row r="134" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="2"/>
@@ -24917,7 +25032,7 @@
       <c r="FD134" s="2"/>
       <c r="FE134" s="2"/>
     </row>
-    <row r="135" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="2"/>
@@ -25080,7 +25195,7 @@
       <c r="FD135" s="2"/>
       <c r="FE135" s="2"/>
     </row>
-    <row r="136" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="2"/>
@@ -25243,7 +25358,7 @@
       <c r="FD136" s="2"/>
       <c r="FE136" s="2"/>
     </row>
-    <row r="137" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="2"/>
@@ -25406,7 +25521,7 @@
       <c r="FD137" s="2"/>
       <c r="FE137" s="2"/>
     </row>
-    <row r="138" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="2"/>
@@ -25569,7 +25684,7 @@
       <c r="FD138" s="2"/>
       <c r="FE138" s="2"/>
     </row>
-    <row r="139" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="2"/>
@@ -25732,7 +25847,7 @@
       <c r="FD139" s="2"/>
       <c r="FE139" s="2"/>
     </row>
-    <row r="140" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="2"/>
@@ -25895,7 +26010,7 @@
       <c r="FD140" s="2"/>
       <c r="FE140" s="2"/>
     </row>
-    <row r="141" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="2"/>
@@ -26058,7 +26173,7 @@
       <c r="FD141" s="2"/>
       <c r="FE141" s="2"/>
     </row>
-    <row r="142" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="2"/>
@@ -26221,7 +26336,7 @@
       <c r="FD142" s="2"/>
       <c r="FE142" s="2"/>
     </row>
-    <row r="143" spans="1:161" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:161" x14ac:dyDescent="0.4">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="2"/>

</xml_diff>